<commit_message>
Scrum Master: Files update
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint1/Burndown chart.xlsx
+++ b/Project_Management/Sprint1/Burndown chart.xlsx
@@ -11,6 +11,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -18,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -63,13 +68,40 @@
     <t>Day 7</t>
   </si>
   <si>
+    <t>Completed Effort</t>
+  </si>
+  <si>
     <t>Remaining Effort</t>
   </si>
   <si>
-    <t>Completed Effort</t>
+    <t>Ideal Burndown</t>
   </si>
   <si>
-    <t>Ideal Burndown</t>
+    <t>Jogar o jogo para conhecer melhor o projeto</t>
+  </si>
+  <si>
+    <t>Dar ideias no servidor de discord e discuti-las</t>
+  </si>
+  <si>
+    <t>Fazer a hierarquia de ficheiros e adiconá-los</t>
+  </si>
+  <si>
+    <t>Fazer fork ao projeto e adicionar os membros ao mesmo</t>
+  </si>
+  <si>
+    <t>Alterar o readme file no repositório git</t>
+  </si>
+  <si>
+    <t>Meeting semanal</t>
+  </si>
+  <si>
+    <t>Fazer servidor de discord para o trabalho e organiza-lo</t>
+  </si>
+  <si>
+    <t>Analisar o código dado</t>
+  </si>
+  <si>
+    <t>Começar a fazer o use case diagram</t>
   </si>
 </sst>
 </file>
@@ -508,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -588,16 +620,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -748,15 +779,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$20:$C$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Completed Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Completed Effort</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -778,10 +801,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -817,8 +840,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="137291264"/>
-        <c:axId val="137292800"/>
+        <c:axId val="169175296"/>
+        <c:axId val="180030848"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -827,15 +850,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$21:$C$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Remaining Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Remaining Effort</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -900,28 +915,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>20</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>15.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>13.000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,15 +952,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$22:$C$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Ideal Burndown</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -995,30 +1002,30 @@
             <c:numRef>
               <c:f>'Burndown Chart'!$D$22:$S$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.142857142857142</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.0">
-                  <c:v>14.285714285714285</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.0">
-                  <c:v>11.428571428571429</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0">
-                  <c:v>8.5714285714285712</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0">
-                  <c:v>5.7142857142857135</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0">
-                  <c:v>2.8571428571428577</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1041,11 +1048,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137291264"/>
-        <c:axId val="137292800"/>
+        <c:axId val="169175296"/>
+        <c:axId val="180030848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137291264"/>
+        <c:axId val="169175296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1095,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137292800"/>
+        <c:crossAx val="180030848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1096,10 +1103,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137292800"/>
+        <c:axId val="180030848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="22"/>
+          <c:max val="30"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1185,7 +1192,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137291264"/>
+        <c:crossAx val="169175296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1849,7 +1856,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2159,7 +2166,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2167,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T31"/>
+  <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,77 +2191,77 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="48"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="47"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="50"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>45220</v>
+        <v>44546</v>
       </c>
       <c r="F4" s="5">
-        <v>45221</v>
+        <v>44547</v>
       </c>
       <c r="G4" s="5">
-        <v>45222</v>
+        <v>44548</v>
       </c>
       <c r="H4" s="5">
-        <v>45223</v>
+        <v>44549</v>
       </c>
       <c r="I4" s="5">
-        <v>45224</v>
+        <v>44550</v>
       </c>
       <c r="J4" s="5">
-        <v>45225</v>
+        <v>44551</v>
       </c>
       <c r="K4" s="5">
-        <v>45226</v>
+        <v>44552</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -2266,8 +2273,8 @@
       <c r="S4" s="5"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2305,12 +2312,18 @@
       <c r="B6" s="30">
         <v>1</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="34">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="33">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -2326,14 +2339,18 @@
       <c r="S6" s="12"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>2</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="35">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="34">
+        <v>2</v>
+      </c>
+      <c r="E7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -2350,14 +2367,18 @@
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="35">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="34">
         <v>2</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="17">
+        <v>2</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -2374,14 +2395,18 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>4</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="35">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="34">
         <v>1</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -2398,15 +2423,19 @@
       <c r="S9" s="16"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>5</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="36">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.1</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14">
+        <v>0.1</v>
+      </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2422,14 +2451,18 @@
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>6</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="36">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19"/>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="35">
+        <v>2</v>
+      </c>
+      <c r="E11" s="19">
+        <v>2</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -2446,14 +2479,18 @@
       <c r="S11" s="16"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>7</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="36">
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="35">
         <v>1</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -2470,12 +2507,14 @@
       <c r="S12" s="16"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="32">
+      <c r="B13" s="31">
         <v>8</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="36">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="35">
+        <v>5</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="14"/>
@@ -2494,12 +2533,14 @@
       <c r="S13" s="16"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>9</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="36">
-        <v>4</v>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="35">
+        <v>5</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="14"/>
@@ -2518,13 +2559,11 @@
       <c r="S14" s="16"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>10</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="36">
-        <v>1</v>
-      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -2542,13 +2581,11 @@
       <c r="S15" s="16"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>11</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="36">
-        <v>2</v>
-      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="19"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -2566,13 +2603,11 @@
       <c r="S16" s="16"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
+      <c r="B17" s="31">
         <v>12</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="36">
-        <v>1</v>
-      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="19"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -2590,13 +2625,11 @@
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="32">
+      <c r="B18" s="31">
         <v>13</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="36">
-        <v>1</v>
-      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="19"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -2613,14 +2646,12 @@
       <c r="R18" s="15"/>
       <c r="S18" s="16"/>
     </row>
-    <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="32">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="31">
         <v>14</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="36">
-        <v>1</v>
-      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="19"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -2638,20 +2669,20 @@
       <c r="S19" s="16"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="53"/>
+      <c r="B20" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="52"/>
       <c r="D20" s="3">
         <v>0</v>
       </c>
       <c r="E20" s="21">
-        <f t="shared" ref="E20:S20" si="0">SUM(E6:E19)</f>
-        <v>0</v>
+        <f t="shared" ref="E20:K20" si="0">SUM(E6:E19)</f>
+        <v>8</v>
       </c>
       <c r="F20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="G20" s="21">
         <f t="shared" si="0"/>
@@ -2680,45 +2711,45 @@
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="29"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="43"/>
+      <c r="B21" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="42"/>
       <c r="D21" s="24">
         <f>SUM(D6:D20)</f>
-        <v>20</v>
+        <v>23.1</v>
       </c>
       <c r="E21" s="25">
-        <f t="shared" ref="E21:S21" si="1">D21-SUM(E6:E19)</f>
-        <v>20</v>
+        <f t="shared" ref="E21:K21" si="1">D21-SUM(E6:E19)</f>
+        <v>15.100000000000001</v>
       </c>
       <c r="F21" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="H21" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -2730,37 +2761,37 @@
       <c r="S21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="26">
         <f>D21</f>
-        <v>20</v>
-      </c>
-      <c r="E22" s="26">
+        <v>23.1</v>
+      </c>
+      <c r="E22" s="27">
         <f>$D$22-($D$22/7*1)</f>
-        <v>17.142857142857142</v>
+        <v>19.8</v>
       </c>
       <c r="F22" s="1">
         <f>$D$22-($D$22/7*2)</f>
-        <v>14.285714285714285</v>
+        <v>16.5</v>
       </c>
       <c r="G22" s="1">
         <f>$D$22-($D$22/7*3)</f>
-        <v>11.428571428571429</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="H22" s="1">
         <f>$D$22-($D$22/7*4)</f>
-        <v>8.5714285714285712</v>
+        <v>9.9</v>
       </c>
       <c r="I22" s="1">
         <f>$D$22-($D$22/7*5)</f>
-        <v>5.7142857142857135</v>
+        <v>6.6000000000000014</v>
       </c>
       <c r="J22" s="1">
         <f>$D$22-($D$22/7*6)</f>
-        <v>2.8571428571428577</v>
+        <v>3.3000000000000007</v>
       </c>
       <c r="K22" s="1">
         <f>$D$22-($D$22/7*7)</f>
@@ -2774,9 +2805,6 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="2"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="S31" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Reversing to my last commit
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint1/Burndown chart.xlsx
+++ b/Project_Management/Sprint1/Burndown chart.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -92,6 +92,9 @@
     <t>Alterar o readme file no repositório git</t>
   </si>
   <si>
+    <t>Meeting semanal</t>
+  </si>
+  <si>
     <t>Fazer servidor de discord para o trabalho e organiza-lo</t>
   </si>
   <si>
@@ -99,12 +102,6 @@
   </si>
   <si>
     <t>Pesquisar como se joga o jogo</t>
-  </si>
-  <si>
-    <t>Meetings</t>
-  </si>
-  <si>
-    <t>Fazer pdf dos 3 User Stories mais votados pela equipa e submeter no moodle</t>
   </si>
 </sst>
 </file>
@@ -816,13 +813,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,8 +840,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="225532160"/>
-        <c:axId val="225550336"/>
+        <c:axId val="232478976"/>
+        <c:axId val="232497152"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -918,28 +915,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>28.6</c:v>
+                  <c:v>25.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.600000000000001</c:v>
+                  <c:v>16.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.5</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.5</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.5</c:v>
+                  <c:v>12.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5</c:v>
+                  <c:v>10.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5</c:v>
+                  <c:v>8.0000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>8.0000000000000018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,25 +1005,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>28.6</c:v>
+                  <c:v>25.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.514285714285716</c:v>
+                  <c:v>21.514285714285716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.428571428571431</c:v>
+                  <c:v>17.928571428571431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.342857142857142</c:v>
+                  <c:v>14.342857142857143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.257142857142856</c:v>
+                  <c:v>10.757142857142858</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.1714285714285708</c:v>
+                  <c:v>7.1714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0857142857142819</c:v>
+                  <c:v>3.5857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1051,11 +1048,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="225532160"/>
-        <c:axId val="225550336"/>
+        <c:axId val="232478976"/>
+        <c:axId val="232497152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="225532160"/>
+        <c:axId val="232478976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1095,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225550336"/>
+        <c:crossAx val="232497152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1106,7 +1103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225550336"/>
+        <c:axId val="232497152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1195,7 +1192,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225532160"/>
+        <c:crossAx val="232478976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,8 +2176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2316,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -2337,9 +2334,7 @@
       <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="K6" s="10">
-        <v>2</v>
-      </c>
+      <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -2371,9 +2366,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="14"/>
-      <c r="K7" s="14">
-        <v>1</v>
-      </c>
+      <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -2472,10 +2465,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="35">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="19">
         <v>2</v>
@@ -2485,9 +2478,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14">
-        <v>1.5</v>
-      </c>
+      <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -2502,7 +2493,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" s="35">
         <v>1</v>
@@ -2530,7 +2521,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="35">
         <v>5</v>
@@ -2539,15 +2530,9 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="14">
-        <v>1</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1</v>
-      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -2562,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="35">
         <v>3</v>
@@ -2577,9 +2562,7 @@
       <c r="J14" s="14">
         <v>1</v>
       </c>
-      <c r="K14" s="14">
-        <v>1</v>
-      </c>
+      <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -2593,21 +2576,15 @@
       <c r="B15" s="31">
         <v>10</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="35">
-        <v>1</v>
-      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="14">
-        <v>1</v>
-      </c>
+      <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
@@ -2731,15 +2708,15 @@
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="21">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2758,35 +2735,35 @@
       <c r="C21" s="42"/>
       <c r="D21" s="24">
         <f>SUM(D6:D20)</f>
-        <v>28.6</v>
+        <v>25.1</v>
       </c>
       <c r="E21" s="25">
         <f t="shared" ref="E21:K21" si="1">D21-SUM(E6:E19)</f>
-        <v>19.600000000000001</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="F21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="H21" s="22">
         <f t="shared" si="1"/>
-        <v>15.5</v>
+        <v>12.000000000000002</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -2804,31 +2781,31 @@
       <c r="C22" s="44"/>
       <c r="D22" s="26">
         <f>D21</f>
-        <v>28.6</v>
+        <v>25.1</v>
       </c>
       <c r="E22" s="27">
         <f>$D$22-($D$22/7*1)</f>
-        <v>24.514285714285716</v>
+        <v>21.514285714285716</v>
       </c>
       <c r="F22" s="1">
         <f>$D$22-($D$22/7*2)</f>
-        <v>20.428571428571431</v>
+        <v>17.928571428571431</v>
       </c>
       <c r="G22" s="1">
         <f>$D$22-($D$22/7*3)</f>
-        <v>16.342857142857142</v>
+        <v>14.342857142857143</v>
       </c>
       <c r="H22" s="1">
         <f>$D$22-($D$22/7*4)</f>
-        <v>12.257142857142856</v>
+        <v>10.757142857142858</v>
       </c>
       <c r="I22" s="1">
         <f>$D$22-($D$22/7*5)</f>
-        <v>8.1714285714285708</v>
+        <v>7.1714285714285708</v>
       </c>
       <c r="J22" s="1">
         <f>$D$22-($D$22/7*6)</f>
-        <v>4.0857142857142819</v>
+        <v>3.5857142857142854</v>
       </c>
       <c r="K22" s="1">
         <f>$D$22-($D$22/7*7)</f>

</xml_diff>

<commit_message>
Fixing wrongly done merge
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint1/Burndown chart.xlsx
+++ b/Project_Management/Sprint1/Burndown chart.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Alterar o readme file no repositório git</t>
   </si>
   <si>
-    <t>Meeting semanal</t>
-  </si>
-  <si>
     <t>Fazer servidor de discord para o trabalho e organiza-lo</t>
   </si>
   <si>
@@ -102,6 +99,12 @@
   </si>
   <si>
     <t>Pesquisar como se joga o jogo</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>Fazer pdf dos 3 User Stories mais votados pela equipa e submeter no moodle</t>
   </si>
 </sst>
 </file>
@@ -813,13 +816,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -840,8 +843,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="232478976"/>
-        <c:axId val="232497152"/>
+        <c:axId val="225532160"/>
+        <c:axId val="225550336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -915,28 +918,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>25.1</c:v>
+                  <c:v>28.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.100000000000001</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.000000000000002</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.000000000000002</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.000000000000002</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.000000000000002</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1005,25 +1008,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>25.1</c:v>
+                  <c:v>28.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.514285714285716</c:v>
+                  <c:v>24.514285714285716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.928571428571431</c:v>
+                  <c:v>20.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.342857142857143</c:v>
+                  <c:v>16.342857142857142</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.757142857142858</c:v>
+                  <c:v>12.257142857142856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.1714285714285708</c:v>
+                  <c:v>8.1714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5857142857142854</c:v>
+                  <c:v>4.0857142857142819</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1048,11 +1051,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="232478976"/>
-        <c:axId val="232497152"/>
+        <c:axId val="225532160"/>
+        <c:axId val="225550336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="232478976"/>
+        <c:axId val="225532160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1098,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232497152"/>
+        <c:crossAx val="225550336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1103,7 +1106,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232497152"/>
+        <c:axId val="225550336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1192,7 +1195,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232478976"/>
+        <c:crossAx val="225532160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2176,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,7 +2319,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -2334,7 +2337,9 @@
       <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -2366,7 +2371,9 @@
         <v>1</v>
       </c>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -2465,10 +2472,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11" s="35">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="E11" s="19">
         <v>2</v>
@@ -2478,7 +2485,9 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="K11" s="14">
+        <v>1.5</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -2493,7 +2502,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="35">
         <v>1</v>
@@ -2521,7 +2530,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="35">
         <v>5</v>
@@ -2530,9 +2539,15 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="I13" s="14">
+        <v>1</v>
+      </c>
+      <c r="J13" s="14">
+        <v>1</v>
+      </c>
+      <c r="K13" s="14">
+        <v>1</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -2547,7 +2562,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="35">
         <v>3</v>
@@ -2562,7 +2577,9 @@
       <c r="J14" s="14">
         <v>1</v>
       </c>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14">
+        <v>1</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -2576,15 +2593,21 @@
       <c r="B15" s="31">
         <v>10</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="35">
+        <v>1</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="K15" s="14">
+        <v>1</v>
+      </c>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
@@ -2708,15 +2731,15 @@
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2735,35 +2758,35 @@
       <c r="C21" s="42"/>
       <c r="D21" s="24">
         <f>SUM(D6:D20)</f>
-        <v>25.1</v>
+        <v>28.6</v>
       </c>
       <c r="E21" s="25">
         <f t="shared" ref="E21:K21" si="1">D21-SUM(E6:E19)</f>
-        <v>16.100000000000001</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F21" s="22">
         <f t="shared" si="1"/>
-        <v>14.000000000000002</v>
+        <v>17.5</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>14.000000000000002</v>
+        <v>17.5</v>
       </c>
       <c r="H21" s="22">
         <f t="shared" si="1"/>
-        <v>12.000000000000002</v>
+        <v>15.5</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="1"/>
-        <v>10.000000000000002</v>
+        <v>12.5</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>8.0000000000000018</v>
+        <v>9.5</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>8.0000000000000018</v>
+        <v>2</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -2781,31 +2804,31 @@
       <c r="C22" s="44"/>
       <c r="D22" s="26">
         <f>D21</f>
-        <v>25.1</v>
+        <v>28.6</v>
       </c>
       <c r="E22" s="27">
         <f>$D$22-($D$22/7*1)</f>
-        <v>21.514285714285716</v>
+        <v>24.514285714285716</v>
       </c>
       <c r="F22" s="1">
         <f>$D$22-($D$22/7*2)</f>
-        <v>17.928571428571431</v>
+        <v>20.428571428571431</v>
       </c>
       <c r="G22" s="1">
         <f>$D$22-($D$22/7*3)</f>
-        <v>14.342857142857143</v>
+        <v>16.342857142857142</v>
       </c>
       <c r="H22" s="1">
         <f>$D$22-($D$22/7*4)</f>
-        <v>10.757142857142858</v>
+        <v>12.257142857142856</v>
       </c>
       <c r="I22" s="1">
         <f>$D$22-($D$22/7*5)</f>
-        <v>7.1714285714285708</v>
+        <v>8.1714285714285708</v>
       </c>
       <c r="J22" s="1">
         <f>$D$22-($D$22/7*6)</f>
-        <v>3.5857142857142854</v>
+        <v>4.0857142857142819</v>
       </c>
       <c r="K22" s="1">
         <f>$D$22-($D$22/7*7)</f>

</xml_diff>